<commit_message>
Include check box to update mapa Re-design table without index add header
</commit_message>
<xml_diff>
--- a/JROROSCO_VOTOS.xlsx
+++ b/JROROSCO_VOTOS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itinfoalvarezandmarsal-my.sharepoint.com/personal/mveiga_alvarezandmarsal_com/Documents/Documents/14_JuniorOrosco/VSCODE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itinfoalvarezandmarsal-my.sharepoint.com/personal/mveiga_alvarezandmarsal_com/Documents/Documents/14_JuniorOrosco/GIT/data_jrorosco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{C0146AF1-B12C-49CC-995E-6B3E2C7AD6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{137F4377-6748-459B-8289-5975E3920AC4}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{C0146AF1-B12C-49CC-995E-6B3E2C7AD6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E024512-6572-43CA-B45C-41F607B67041}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{003D9356-3373-4D97-AC59-0FF3F6B48079}"/>
   </bookViews>
@@ -36,40 +36,40 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>PERC</t>
-  </si>
-  <si>
     <t>LAT</t>
   </si>
   <si>
     <t>LONG</t>
   </si>
   <si>
-    <t>NM_LOCALIDADE</t>
+    <t>Mauá</t>
+  </si>
+  <si>
+    <t>Poá</t>
+  </si>
+  <si>
+    <t>Ribeirão Pires</t>
+  </si>
+  <si>
+    <t>Santo André</t>
+  </si>
+  <si>
+    <t>Suzano</t>
+  </si>
+  <si>
+    <t>Nome da Localidade</t>
+  </si>
+  <si>
+    <t>Percentual</t>
+  </si>
+  <si>
+    <t>Total pesquia</t>
+  </si>
+  <si>
+    <t>Votos</t>
   </si>
   <si>
     <t>São Paulo</t>
-  </si>
-  <si>
-    <t>Mauá</t>
-  </si>
-  <si>
-    <t>Poá</t>
-  </si>
-  <si>
-    <t>Ribeirão Pires</t>
-  </si>
-  <si>
-    <t>Santo André</t>
-  </si>
-  <si>
-    <t>Suzano</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>VOTOS</t>
   </si>
 </sst>
 </file>
@@ -439,12 +439,12 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
@@ -452,27 +452,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
         <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3">
         <v>-46.494898793685003</v>
@@ -493,7 +493,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>-46.458262012164703</v>
@@ -514,7 +514,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>-46.346220388658701</v>
@@ -535,7 +535,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>-46.415344374918497</v>
@@ -556,7 +556,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>-46.530874257629499</v>
@@ -577,7 +577,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>-46.307810467288199</v>

</xml_diff>

<commit_message>
fix error strtig "Total Pesquisa"
</commit_message>
<xml_diff>
--- a/JROROSCO_VOTOS.xlsx
+++ b/JROROSCO_VOTOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itinfoalvarezandmarsal-my.sharepoint.com/personal/mveiga_alvarezandmarsal_com/Documents/Documents/14_JuniorOrosco/GIT/data_jrorosco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{C0146AF1-B12C-49CC-995E-6B3E2C7AD6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E024512-6572-43CA-B45C-41F607B67041}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{C0146AF1-B12C-49CC-995E-6B3E2C7AD6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{081D4DF9-128D-46E9-BD10-4F77E4946435}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{003D9356-3373-4D97-AC59-0FF3F6B48079}"/>
   </bookViews>
@@ -63,13 +63,13 @@
     <t>Percentual</t>
   </si>
   <si>
-    <t>Total pesquia</t>
-  </si>
-  <si>
     <t>Votos</t>
   </si>
   <si>
     <t>São Paulo</t>
+  </si>
+  <si>
+    <t>Total pesquisa</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -464,15 +464,15 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3">
         <v>-46.494898793685003</v>

</xml_diff>